<commit_message>
DOCS AND SLIDES UPDATE
</commit_message>
<xml_diff>
--- a/190874H_IWP_DOCS/190874H_Gantt_Chart.xlsx
+++ b/190874H_IWP_DOCS/190874H_Gantt_Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B87097EE-BD5A-4DE9-A550-B4175CCACD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6345F99B-49EB-475D-87BF-54CB6625285A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,22 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -136,9 +121,6 @@
   </si>
   <si>
     <t>Enter Company Name in cell B2.</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -242,6 +224,27 @@
   </si>
   <si>
     <t>Power-ups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passive skills </t>
+  </si>
+  <si>
+    <t>Sound system</t>
+  </si>
+  <si>
+    <t>Highscore</t>
+  </si>
+  <si>
+    <t>Better/improved UI</t>
+  </si>
+  <si>
+    <t>Local play input system</t>
+  </si>
+  <si>
+    <t>Particle effects</t>
+  </si>
+  <si>
+    <t>Improved enemies</t>
   </si>
 </sst>
 </file>
@@ -501,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -621,6 +624,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -652,7 +681,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -887,7 +916,10 @@
     <xf numFmtId="167" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="3" xfId="9">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="11" xfId="9" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="12" xfId="9" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -906,7 +938,145 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="25">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1033,15 +1203,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="11"/>
-      <tableStyleElement type="headerRow" dxfId="10"/>
-      <tableStyleElement type="totalRow" dxfId="9"/>
-      <tableStyleElement type="firstColumn" dxfId="8"/>
-      <tableStyleElement type="lastColumn" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="secondRowStripe" dxfId="5"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="3"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="totalRow" dxfId="22"/>
+      <tableStyleElement type="firstColumn" dxfId="21"/>
+      <tableStyleElement type="lastColumn" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="secondRowStripe" dxfId="18"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="16"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1456,11 +1626,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BL39"/>
+  <dimension ref="A1:DI36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BO15" sqref="BO15:BP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1473,16 +1643,17 @@
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
     <col min="7" max="7" width="2.7109375" customWidth="1"/>
     <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5703125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="9" max="72" width="2.5703125" customWidth="1"/>
+    <col min="73" max="73" width="1.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="113" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:113" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="54" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1491,35 +1662,62 @@
       <c r="H1" s="2"/>
       <c r="I1" s="76"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:113" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="58"/>
       <c r="I2" s="77"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:113" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="53" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C3" s="79" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3" s="80"/>
       <c r="E3" s="84">
         <v>44865</v>
       </c>
-      <c r="F3" s="84"/>
+      <c r="F3" s="85"/>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AG3">
+        <v>4</v>
+      </c>
+      <c r="AN3">
+        <v>5</v>
+      </c>
+      <c r="AT3">
+        <v>6</v>
+      </c>
+      <c r="BB3">
+        <v>7</v>
+      </c>
+      <c r="BJ3">
+        <v>8</v>
+      </c>
+      <c r="BO3">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:113" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="80"/>
       <c r="E4" s="7">
@@ -1605,10 +1803,80 @@
       <c r="BJ4" s="82"/>
       <c r="BK4" s="82"/>
       <c r="BL4" s="83"/>
+      <c r="BM4" s="81">
+        <f>BM5</f>
+        <v>44921</v>
+      </c>
+      <c r="BN4" s="82"/>
+      <c r="BO4" s="82"/>
+      <c r="BP4" s="82"/>
+      <c r="BQ4" s="82"/>
+      <c r="BR4" s="82"/>
+      <c r="BS4" s="83"/>
+      <c r="BT4" s="81">
+        <f>BT5</f>
+        <v>44928</v>
+      </c>
+      <c r="BU4" s="82"/>
+      <c r="BV4" s="82"/>
+      <c r="BW4" s="82"/>
+      <c r="BX4" s="82"/>
+      <c r="BY4" s="82"/>
+      <c r="BZ4" s="83"/>
+      <c r="CA4" s="81">
+        <f>CA5</f>
+        <v>44935</v>
+      </c>
+      <c r="CB4" s="82"/>
+      <c r="CC4" s="82"/>
+      <c r="CD4" s="82"/>
+      <c r="CE4" s="82"/>
+      <c r="CF4" s="82"/>
+      <c r="CG4" s="83"/>
+      <c r="CH4" s="81">
+        <f>CH5</f>
+        <v>44942</v>
+      </c>
+      <c r="CI4" s="82"/>
+      <c r="CJ4" s="82"/>
+      <c r="CK4" s="82"/>
+      <c r="CL4" s="82"/>
+      <c r="CM4" s="82"/>
+      <c r="CN4" s="83"/>
+      <c r="CO4" s="81">
+        <f>CO5</f>
+        <v>44949</v>
+      </c>
+      <c r="CP4" s="82"/>
+      <c r="CQ4" s="82"/>
+      <c r="CR4" s="82"/>
+      <c r="CS4" s="82"/>
+      <c r="CT4" s="82"/>
+      <c r="CU4" s="83"/>
+      <c r="CV4" s="81">
+        <f>CV5</f>
+        <v>44956</v>
+      </c>
+      <c r="CW4" s="82"/>
+      <c r="CX4" s="82"/>
+      <c r="CY4" s="82"/>
+      <c r="CZ4" s="82"/>
+      <c r="DA4" s="82"/>
+      <c r="DB4" s="83"/>
+      <c r="DC4" s="81">
+        <f>DC5</f>
+        <v>44963</v>
+      </c>
+      <c r="DD4" s="82"/>
+      <c r="DE4" s="82"/>
+      <c r="DF4" s="82"/>
+      <c r="DG4" s="82"/>
+      <c r="DH4" s="82"/>
+      <c r="DI4" s="83"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B5" s="75"/>
       <c r="C5" s="75"/>
@@ -1840,258 +2108,650 @@
         <f t="shared" si="2"/>
         <v>44920</v>
       </c>
+      <c r="BM5" s="11">
+        <f>BL5+1</f>
+        <v>44921</v>
+      </c>
+      <c r="BN5" s="10">
+        <f>BM5+1</f>
+        <v>44922</v>
+      </c>
+      <c r="BO5" s="10">
+        <f t="shared" ref="BO5" si="3">BN5+1</f>
+        <v>44923</v>
+      </c>
+      <c r="BP5" s="10">
+        <f t="shared" ref="BP5" si="4">BO5+1</f>
+        <v>44924</v>
+      </c>
+      <c r="BQ5" s="10">
+        <f t="shared" ref="BQ5" si="5">BP5+1</f>
+        <v>44925</v>
+      </c>
+      <c r="BR5" s="10">
+        <f t="shared" ref="BR5" si="6">BQ5+1</f>
+        <v>44926</v>
+      </c>
+      <c r="BS5" s="12">
+        <f t="shared" ref="BS5" si="7">BR5+1</f>
+        <v>44927</v>
+      </c>
+      <c r="BT5" s="11">
+        <f>BS5+1</f>
+        <v>44928</v>
+      </c>
+      <c r="BU5" s="10">
+        <f>BT5+1</f>
+        <v>44929</v>
+      </c>
+      <c r="BV5" s="10">
+        <f t="shared" ref="BV5" si="8">BU5+1</f>
+        <v>44930</v>
+      </c>
+      <c r="BW5" s="10">
+        <f t="shared" ref="BW5" si="9">BV5+1</f>
+        <v>44931</v>
+      </c>
+      <c r="BX5" s="10">
+        <f t="shared" ref="BX5" si="10">BW5+1</f>
+        <v>44932</v>
+      </c>
+      <c r="BY5" s="10">
+        <f t="shared" ref="BY5" si="11">BX5+1</f>
+        <v>44933</v>
+      </c>
+      <c r="BZ5" s="12">
+        <f t="shared" ref="BZ5" si="12">BY5+1</f>
+        <v>44934</v>
+      </c>
+      <c r="CA5" s="11">
+        <f>BZ5+1</f>
+        <v>44935</v>
+      </c>
+      <c r="CB5" s="10">
+        <f>CA5+1</f>
+        <v>44936</v>
+      </c>
+      <c r="CC5" s="10">
+        <f t="shared" ref="CC5" si="13">CB5+1</f>
+        <v>44937</v>
+      </c>
+      <c r="CD5" s="10">
+        <f t="shared" ref="CD5" si="14">CC5+1</f>
+        <v>44938</v>
+      </c>
+      <c r="CE5" s="10">
+        <f t="shared" ref="CE5" si="15">CD5+1</f>
+        <v>44939</v>
+      </c>
+      <c r="CF5" s="10">
+        <f t="shared" ref="CF5" si="16">CE5+1</f>
+        <v>44940</v>
+      </c>
+      <c r="CG5" s="12">
+        <f t="shared" ref="CG5" si="17">CF5+1</f>
+        <v>44941</v>
+      </c>
+      <c r="CH5" s="11">
+        <f>CG5+1</f>
+        <v>44942</v>
+      </c>
+      <c r="CI5" s="10">
+        <f>CH5+1</f>
+        <v>44943</v>
+      </c>
+      <c r="CJ5" s="10">
+        <f t="shared" ref="CJ5" si="18">CI5+1</f>
+        <v>44944</v>
+      </c>
+      <c r="CK5" s="10">
+        <f t="shared" ref="CK5" si="19">CJ5+1</f>
+        <v>44945</v>
+      </c>
+      <c r="CL5" s="10">
+        <f t="shared" ref="CL5" si="20">CK5+1</f>
+        <v>44946</v>
+      </c>
+      <c r="CM5" s="10">
+        <f t="shared" ref="CM5" si="21">CL5+1</f>
+        <v>44947</v>
+      </c>
+      <c r="CN5" s="12">
+        <f t="shared" ref="CN5" si="22">CM5+1</f>
+        <v>44948</v>
+      </c>
+      <c r="CO5" s="11">
+        <f>CN5+1</f>
+        <v>44949</v>
+      </c>
+      <c r="CP5" s="10">
+        <f>CO5+1</f>
+        <v>44950</v>
+      </c>
+      <c r="CQ5" s="10">
+        <f t="shared" ref="CQ5" si="23">CP5+1</f>
+        <v>44951</v>
+      </c>
+      <c r="CR5" s="10">
+        <f t="shared" ref="CR5" si="24">CQ5+1</f>
+        <v>44952</v>
+      </c>
+      <c r="CS5" s="10">
+        <f t="shared" ref="CS5" si="25">CR5+1</f>
+        <v>44953</v>
+      </c>
+      <c r="CT5" s="10">
+        <f t="shared" ref="CT5" si="26">CS5+1</f>
+        <v>44954</v>
+      </c>
+      <c r="CU5" s="12">
+        <f t="shared" ref="CU5" si="27">CT5+1</f>
+        <v>44955</v>
+      </c>
+      <c r="CV5" s="11">
+        <f>CU5+1</f>
+        <v>44956</v>
+      </c>
+      <c r="CW5" s="10">
+        <f>CV5+1</f>
+        <v>44957</v>
+      </c>
+      <c r="CX5" s="10">
+        <f t="shared" ref="CX5" si="28">CW5+1</f>
+        <v>44958</v>
+      </c>
+      <c r="CY5" s="10">
+        <f t="shared" ref="CY5" si="29">CX5+1</f>
+        <v>44959</v>
+      </c>
+      <c r="CZ5" s="10">
+        <f t="shared" ref="CZ5" si="30">CY5+1</f>
+        <v>44960</v>
+      </c>
+      <c r="DA5" s="10">
+        <f t="shared" ref="DA5" si="31">CZ5+1</f>
+        <v>44961</v>
+      </c>
+      <c r="DB5" s="12">
+        <f t="shared" ref="DB5" si="32">DA5+1</f>
+        <v>44962</v>
+      </c>
+      <c r="DC5" s="11">
+        <f>DB5+1</f>
+        <v>44963</v>
+      </c>
+      <c r="DD5" s="10">
+        <f>DC5+1</f>
+        <v>44964</v>
+      </c>
+      <c r="DE5" s="10">
+        <f t="shared" ref="DE5" si="33">DD5+1</f>
+        <v>44965</v>
+      </c>
+      <c r="DF5" s="10">
+        <f t="shared" ref="DF5" si="34">DE5+1</f>
+        <v>44966</v>
+      </c>
+      <c r="DG5" s="10">
+        <f t="shared" ref="DG5" si="35">DF5+1</f>
+        <v>44967</v>
+      </c>
+      <c r="DH5" s="10">
+        <f>DG5+1</f>
+        <v>44968</v>
+      </c>
+      <c r="DI5" s="12">
+        <f t="shared" ref="DI5" si="36">DH5+1</f>
+        <v>44969</v>
+      </c>
     </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:113" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="54" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6" si="37">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f t="shared" ref="J6:AR6" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AR6" si="38">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>W</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>F</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>M</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>W</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>F</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>M</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>W</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>F</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="AD6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>M</v>
       </c>
       <c r="AE6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="AF6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>W</v>
       </c>
       <c r="AG6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="AH6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>F</v>
       </c>
       <c r="AI6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="AJ6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="AK6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>M</v>
       </c>
       <c r="AL6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="AM6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>W</v>
       </c>
       <c r="AN6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>T</v>
       </c>
       <c r="AO6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>F</v>
       </c>
       <c r="AP6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="AQ6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>S</v>
       </c>
       <c r="AR6" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="38"/>
         <v>M</v>
       </c>
       <c r="AS6" s="13" t="str">
-        <f t="shared" ref="AS6:BL6" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <f t="shared" ref="AS6:BL6" si="39">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AT6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>W</v>
       </c>
       <c r="AU6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>T</v>
       </c>
       <c r="AV6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>F</v>
       </c>
       <c r="AW6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>S</v>
       </c>
       <c r="AX6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>S</v>
       </c>
       <c r="AY6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>M</v>
       </c>
       <c r="AZ6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>T</v>
       </c>
       <c r="BA6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>W</v>
       </c>
       <c r="BB6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>T</v>
       </c>
       <c r="BC6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>F</v>
       </c>
       <c r="BD6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>S</v>
       </c>
       <c r="BE6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>S</v>
       </c>
       <c r="BF6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>M</v>
       </c>
       <c r="BG6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>T</v>
       </c>
       <c r="BH6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>W</v>
       </c>
       <c r="BI6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>T</v>
       </c>
       <c r="BJ6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>F</v>
       </c>
       <c r="BK6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>S</v>
       </c>
       <c r="BL6" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="39"/>
         <v>S</v>
       </c>
+      <c r="BM6" s="13" t="str">
+        <f t="shared" ref="BM6:BZ6" si="40">LEFT(TEXT(BM5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="BN6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>T</v>
+      </c>
+      <c r="BO6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>W</v>
+      </c>
+      <c r="BP6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>T</v>
+      </c>
+      <c r="BQ6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>F</v>
+      </c>
+      <c r="BR6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>S</v>
+      </c>
+      <c r="BS6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>S</v>
+      </c>
+      <c r="BT6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>M</v>
+      </c>
+      <c r="BU6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>T</v>
+      </c>
+      <c r="BV6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>W</v>
+      </c>
+      <c r="BW6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>T</v>
+      </c>
+      <c r="BX6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>F</v>
+      </c>
+      <c r="BY6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>S</v>
+      </c>
+      <c r="BZ6" s="13" t="str">
+        <f t="shared" si="40"/>
+        <v>S</v>
+      </c>
+      <c r="CA6" s="13" t="str">
+        <f t="shared" ref="CA6:CN6" si="41">LEFT(TEXT(CA5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="CB6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>T</v>
+      </c>
+      <c r="CC6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>W</v>
+      </c>
+      <c r="CD6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>T</v>
+      </c>
+      <c r="CE6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>F</v>
+      </c>
+      <c r="CF6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>S</v>
+      </c>
+      <c r="CG6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>S</v>
+      </c>
+      <c r="CH6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>M</v>
+      </c>
+      <c r="CI6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>T</v>
+      </c>
+      <c r="CJ6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>W</v>
+      </c>
+      <c r="CK6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>T</v>
+      </c>
+      <c r="CL6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>F</v>
+      </c>
+      <c r="CM6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>S</v>
+      </c>
+      <c r="CN6" s="13" t="str">
+        <f t="shared" si="41"/>
+        <v>S</v>
+      </c>
+      <c r="CO6" s="13" t="str">
+        <f t="shared" ref="CO6:DB6" si="42">LEFT(TEXT(CO5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="CP6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>T</v>
+      </c>
+      <c r="CQ6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>W</v>
+      </c>
+      <c r="CR6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>T</v>
+      </c>
+      <c r="CS6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>F</v>
+      </c>
+      <c r="CT6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>S</v>
+      </c>
+      <c r="CU6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>S</v>
+      </c>
+      <c r="CV6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>M</v>
+      </c>
+      <c r="CW6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>T</v>
+      </c>
+      <c r="CX6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>W</v>
+      </c>
+      <c r="CY6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>T</v>
+      </c>
+      <c r="CZ6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>F</v>
+      </c>
+      <c r="DA6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>S</v>
+      </c>
+      <c r="DB6" s="13" t="str">
+        <f t="shared" si="42"/>
+        <v>S</v>
+      </c>
+      <c r="DC6" s="13" t="str">
+        <f t="shared" ref="DC6:DI6" si="43">LEFT(TEXT(DC5,"ddd"),1)</f>
+        <v>M</v>
+      </c>
+      <c r="DD6" s="13" t="str">
+        <f t="shared" si="43"/>
+        <v>T</v>
+      </c>
+      <c r="DE6" s="13" t="str">
+        <f t="shared" si="43"/>
+        <v>W</v>
+      </c>
+      <c r="DF6" s="13" t="str">
+        <f t="shared" si="43"/>
+        <v>T</v>
+      </c>
+      <c r="DG6" s="13" t="str">
+        <f t="shared" si="43"/>
+        <v>F</v>
+      </c>
+      <c r="DH6" s="13" t="str">
+        <f t="shared" si="43"/>
+        <v>S</v>
+      </c>
+      <c r="DI6" s="13" t="str">
+        <f t="shared" si="43"/>
+        <v>S</v>
+      </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:113" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="53" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C7" s="56"/>
       <c r="E7"/>
@@ -2156,12 +2816,12 @@
       <c r="BK7" s="39"/>
       <c r="BL7" s="39"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="54" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C8" s="64"/>
       <c r="D8" s="19"/>
@@ -2169,7 +2829,7 @@
       <c r="F8" s="21"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17" t="str">
-        <f t="shared" ref="H8:H36" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H33" si="44">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="39"/>
@@ -2228,32 +2888,79 @@
       <c r="BJ8" s="39"/>
       <c r="BK8" s="39"/>
       <c r="BL8" s="39"/>
+      <c r="BM8" s="39"/>
+      <c r="BN8" s="39"/>
+      <c r="BO8" s="39"/>
+      <c r="BP8" s="39"/>
+      <c r="BQ8" s="39"/>
+      <c r="BR8" s="39"/>
+      <c r="BS8" s="39"/>
+      <c r="BT8" s="39"/>
+      <c r="BU8" s="39"/>
+      <c r="BV8" s="39"/>
+      <c r="BW8" s="39"/>
+      <c r="BX8" s="39"/>
+      <c r="BY8" s="39"/>
+      <c r="BZ8" s="39"/>
+      <c r="CA8" s="39"/>
+      <c r="CB8" s="39"/>
+      <c r="CC8" s="39"/>
+      <c r="CD8" s="39"/>
+      <c r="CE8" s="39"/>
+      <c r="CF8" s="39"/>
+      <c r="CG8" s="39"/>
+      <c r="CH8" s="39"/>
+      <c r="CI8" s="39"/>
+      <c r="CJ8" s="39"/>
+      <c r="CK8" s="39"/>
+      <c r="CL8" s="39"/>
+      <c r="CM8" s="39"/>
+      <c r="CN8" s="39"/>
+      <c r="CO8" s="39"/>
+      <c r="CP8" s="39"/>
+      <c r="CQ8" s="39"/>
+      <c r="CR8" s="39"/>
+      <c r="CS8" s="39"/>
+      <c r="CT8" s="39"/>
+      <c r="CU8" s="39"/>
+      <c r="CV8" s="39"/>
+      <c r="CW8" s="39"/>
+      <c r="CX8" s="39"/>
+      <c r="CY8" s="39"/>
+      <c r="CZ8" s="39"/>
+      <c r="DA8" s="39"/>
+      <c r="DB8" s="39"/>
+      <c r="DC8" s="39"/>
+      <c r="DD8" s="39"/>
+      <c r="DE8" s="39"/>
+      <c r="DF8" s="39"/>
+      <c r="DG8" s="39"/>
+      <c r="DH8" s="39"/>
+      <c r="DI8" s="39"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="54" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B9" s="71" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>30</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C9" s="65"/>
       <c r="D9" s="22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E9" s="60">
         <f>Project_Start</f>
         <v>44865</v>
       </c>
       <c r="F9" s="60">
-        <f>E9+3</f>
-        <v>44868</v>
+        <f>E9+10</f>
+        <v>44875</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="44"/>
+        <v>11</v>
       </c>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
@@ -2311,31 +3018,75 @@
       <c r="BJ9" s="39"/>
       <c r="BK9" s="39"/>
       <c r="BL9" s="39"/>
+      <c r="BM9" s="39"/>
+      <c r="BN9" s="39"/>
+      <c r="BO9" s="39"/>
+      <c r="BP9" s="39"/>
+      <c r="BQ9" s="39"/>
+      <c r="BR9" s="39"/>
+      <c r="BS9" s="39"/>
+      <c r="BT9" s="39"/>
+      <c r="BU9" s="39"/>
+      <c r="BV9" s="39"/>
+      <c r="BW9" s="39"/>
+      <c r="BX9" s="39"/>
+      <c r="BY9" s="39"/>
+      <c r="BZ9" s="39"/>
+      <c r="CA9" s="39"/>
+      <c r="CB9" s="39"/>
+      <c r="CC9" s="39"/>
+      <c r="CD9" s="39"/>
+      <c r="CE9" s="39"/>
+      <c r="CF9" s="39"/>
+      <c r="CG9" s="39"/>
+      <c r="CH9" s="39"/>
+      <c r="CI9" s="39"/>
+      <c r="CJ9" s="39"/>
+      <c r="CK9" s="39"/>
+      <c r="CL9" s="39"/>
+      <c r="CM9" s="39"/>
+      <c r="CN9" s="39"/>
+      <c r="CO9" s="39"/>
+      <c r="CP9" s="39"/>
+      <c r="CQ9" s="39"/>
+      <c r="CR9" s="39"/>
+      <c r="CS9" s="39"/>
+      <c r="CT9" s="39"/>
+      <c r="CU9" s="39"/>
+      <c r="CV9" s="39"/>
+      <c r="CW9" s="39"/>
+      <c r="CX9" s="39"/>
+      <c r="CY9" s="39"/>
+      <c r="CZ9" s="39"/>
+      <c r="DA9" s="39"/>
+      <c r="DB9" s="39"/>
+      <c r="DC9" s="39"/>
+      <c r="DD9" s="39"/>
+      <c r="DE9" s="39"/>
+      <c r="DF9" s="39"/>
+      <c r="DG9" s="39"/>
+      <c r="DH9" s="39"/>
+      <c r="DI9" s="39"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="54" t="s">
-        <v>39</v>
-      </c>
+    <row r="10" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="54"/>
       <c r="B10" s="71" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="65"/>
       <c r="D10" s="22">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E10" s="60">
         <f>F9</f>
-        <v>44868</v>
+        <v>44875</v>
       </c>
       <c r="F10" s="60">
-        <f>E10+2</f>
-        <v>44870</v>
+        <f>E9+23</f>
+        <v>44888</v>
       </c>
       <c r="G10" s="17"/>
-      <c r="H10" s="17">
-        <f t="shared" si="6"/>
-        <v>3</v>
-      </c>
+      <c r="H10" s="17"/>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
@@ -2348,8 +3099,8 @@
       <c r="R10" s="39"/>
       <c r="S10" s="39"/>
       <c r="T10" s="39"/>
-      <c r="U10" s="40"/>
-      <c r="V10" s="40"/>
+      <c r="U10" s="39"/>
+      <c r="V10" s="39"/>
       <c r="W10" s="39"/>
       <c r="X10" s="39"/>
       <c r="Y10" s="39"/>
@@ -2392,28 +3143,79 @@
       <c r="BJ10" s="39"/>
       <c r="BK10" s="39"/>
       <c r="BL10" s="39"/>
+      <c r="BM10" s="39"/>
+      <c r="BN10" s="39"/>
+      <c r="BO10" s="39"/>
+      <c r="BP10" s="39"/>
+      <c r="BQ10" s="39"/>
+      <c r="BR10" s="39"/>
+      <c r="BS10" s="39"/>
+      <c r="BT10" s="39"/>
+      <c r="BU10" s="39"/>
+      <c r="BV10" s="39"/>
+      <c r="BW10" s="39"/>
+      <c r="BX10" s="39"/>
+      <c r="BY10" s="39"/>
+      <c r="BZ10" s="39"/>
+      <c r="CA10" s="39"/>
+      <c r="CB10" s="39"/>
+      <c r="CC10" s="39"/>
+      <c r="CD10" s="39"/>
+      <c r="CE10" s="39"/>
+      <c r="CF10" s="39"/>
+      <c r="CG10" s="39"/>
+      <c r="CH10" s="39"/>
+      <c r="CI10" s="39"/>
+      <c r="CJ10" s="39"/>
+      <c r="CK10" s="39"/>
+      <c r="CL10" s="39"/>
+      <c r="CM10" s="39"/>
+      <c r="CN10" s="39"/>
+      <c r="CO10" s="39"/>
+      <c r="CP10" s="39"/>
+      <c r="CQ10" s="39"/>
+      <c r="CR10" s="39"/>
+      <c r="CS10" s="39"/>
+      <c r="CT10" s="39"/>
+      <c r="CU10" s="39"/>
+      <c r="CV10" s="39"/>
+      <c r="CW10" s="39"/>
+      <c r="CX10" s="39"/>
+      <c r="CY10" s="39"/>
+      <c r="CZ10" s="39"/>
+      <c r="DA10" s="39"/>
+      <c r="DB10" s="39"/>
+      <c r="DC10" s="39"/>
+      <c r="DD10" s="39"/>
+      <c r="DE10" s="39"/>
+      <c r="DF10" s="39"/>
+      <c r="DG10" s="39"/>
+      <c r="DH10" s="39"/>
+      <c r="DI10" s="39"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="53"/>
+    <row r="11" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="54" t="s">
+        <v>33</v>
+      </c>
       <c r="B11" s="71" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C11" s="65"/>
       <c r="D11" s="22">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E11" s="60">
         <f>F10</f>
-        <v>44870</v>
+        <v>44888</v>
       </c>
       <c r="F11" s="60">
-        <f>E11+4</f>
-        <v>44874</v>
+        <f>E11+5</f>
+        <v>44893</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="44"/>
+        <v>6</v>
       </c>
       <c r="I11" s="39"/>
       <c r="J11" s="39"/>
@@ -2427,8 +3229,8 @@
       <c r="R11" s="39"/>
       <c r="S11" s="39"/>
       <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="40"/>
       <c r="W11" s="39"/>
       <c r="X11" s="39"/>
       <c r="Y11" s="39"/>
@@ -2471,28 +3273,77 @@
       <c r="BJ11" s="39"/>
       <c r="BK11" s="39"/>
       <c r="BL11" s="39"/>
+      <c r="BM11" s="39"/>
+      <c r="BN11" s="39"/>
+      <c r="BO11" s="39"/>
+      <c r="BP11" s="39"/>
+      <c r="BQ11" s="39"/>
+      <c r="BR11" s="39"/>
+      <c r="BS11" s="39"/>
+      <c r="BT11" s="39"/>
+      <c r="BU11" s="39"/>
+      <c r="BV11" s="39"/>
+      <c r="BW11" s="39"/>
+      <c r="BX11" s="39"/>
+      <c r="BY11" s="39"/>
+      <c r="BZ11" s="39"/>
+      <c r="CA11" s="39"/>
+      <c r="CB11" s="39"/>
+      <c r="CC11" s="39"/>
+      <c r="CD11" s="39"/>
+      <c r="CE11" s="39"/>
+      <c r="CF11" s="39"/>
+      <c r="CG11" s="39"/>
+      <c r="CH11" s="39"/>
+      <c r="CI11" s="39"/>
+      <c r="CJ11" s="39"/>
+      <c r="CK11" s="39"/>
+      <c r="CL11" s="39"/>
+      <c r="CM11" s="39"/>
+      <c r="CN11" s="39"/>
+      <c r="CO11" s="39"/>
+      <c r="CP11" s="39"/>
+      <c r="CQ11" s="39"/>
+      <c r="CR11" s="39"/>
+      <c r="CS11" s="39"/>
+      <c r="CT11" s="39"/>
+      <c r="CU11" s="39"/>
+      <c r="CV11" s="39"/>
+      <c r="CW11" s="39"/>
+      <c r="CX11" s="39"/>
+      <c r="CY11" s="39"/>
+      <c r="CZ11" s="39"/>
+      <c r="DA11" s="39"/>
+      <c r="DB11" s="39"/>
+      <c r="DC11" s="39"/>
+      <c r="DD11" s="39"/>
+      <c r="DE11" s="39"/>
+      <c r="DF11" s="39"/>
+      <c r="DG11" s="39"/>
+      <c r="DH11" s="39"/>
+      <c r="DI11" s="39"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="53"/>
       <c r="B12" s="71" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C12" s="65"/>
       <c r="D12" s="22">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E12" s="60">
         <f>F11</f>
-        <v>44874</v>
+        <v>44893</v>
       </c>
       <c r="F12" s="60">
-        <f>E12+5</f>
-        <v>44879</v>
+        <f>E12+15</f>
+        <v>44908</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17">
-        <f t="shared" si="6"/>
-        <v>6</v>
+        <f t="shared" si="44"/>
+        <v>16</v>
       </c>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
@@ -2510,7 +3361,7 @@
       <c r="V12" s="39"/>
       <c r="W12" s="39"/>
       <c r="X12" s="39"/>
-      <c r="Y12" s="40"/>
+      <c r="Y12" s="39"/>
       <c r="Z12" s="39"/>
       <c r="AA12" s="39"/>
       <c r="AB12" s="39"/>
@@ -2550,16 +3401,78 @@
       <c r="BJ12" s="39"/>
       <c r="BK12" s="39"/>
       <c r="BL12" s="39"/>
+      <c r="BM12" s="39"/>
+      <c r="BN12" s="39"/>
+      <c r="BO12" s="39"/>
+      <c r="BP12" s="39"/>
+      <c r="BQ12" s="39"/>
+      <c r="BR12" s="39"/>
+      <c r="BS12" s="39"/>
+      <c r="BT12" s="39"/>
+      <c r="BU12" s="39"/>
+      <c r="BV12" s="39"/>
+      <c r="BW12" s="39"/>
+      <c r="BX12" s="39"/>
+      <c r="BY12" s="39"/>
+      <c r="BZ12" s="39"/>
+      <c r="CA12" s="39"/>
+      <c r="CB12" s="39"/>
+      <c r="CC12" s="39"/>
+      <c r="CD12" s="39"/>
+      <c r="CE12" s="39"/>
+      <c r="CF12" s="39"/>
+      <c r="CG12" s="39"/>
+      <c r="CH12" s="39"/>
+      <c r="CI12" s="39"/>
+      <c r="CJ12" s="39"/>
+      <c r="CK12" s="39"/>
+      <c r="CL12" s="39"/>
+      <c r="CM12" s="39"/>
+      <c r="CN12" s="39"/>
+      <c r="CO12" s="39"/>
+      <c r="CP12" s="39"/>
+      <c r="CQ12" s="39"/>
+      <c r="CR12" s="39"/>
+      <c r="CS12" s="39"/>
+      <c r="CT12" s="39"/>
+      <c r="CU12" s="39"/>
+      <c r="CV12" s="39"/>
+      <c r="CW12" s="39"/>
+      <c r="CX12" s="39"/>
+      <c r="CY12" s="39"/>
+      <c r="CZ12" s="39"/>
+      <c r="DA12" s="39"/>
+      <c r="DB12" s="39"/>
+      <c r="DC12" s="39"/>
+      <c r="DD12" s="39"/>
+      <c r="DE12" s="39"/>
+      <c r="DF12" s="39"/>
+      <c r="DG12" s="39"/>
+      <c r="DH12" s="39"/>
+      <c r="DI12" s="39"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="53"/>
-      <c r="B13" s="71"/>
+      <c r="B13" s="71" t="s">
+        <v>46</v>
+      </c>
       <c r="C13" s="65"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
+      <c r="D13" s="22">
+        <v>0</v>
+      </c>
+      <c r="E13" s="60">
+        <f>F12</f>
+        <v>44908</v>
+      </c>
+      <c r="F13" s="60">
+        <f>E13+5</f>
+        <v>44913</v>
+      </c>
       <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
+      <c r="H13" s="17">
+        <f t="shared" si="44"/>
+        <v>6</v>
+      </c>
       <c r="I13" s="39"/>
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
@@ -2616,16 +3529,72 @@
       <c r="BJ13" s="39"/>
       <c r="BK13" s="39"/>
       <c r="BL13" s="39"/>
+      <c r="BM13" s="39"/>
+      <c r="BN13" s="39"/>
+      <c r="BO13" s="39"/>
+      <c r="BP13" s="39"/>
+      <c r="BQ13" s="39"/>
+      <c r="BR13" s="39"/>
+      <c r="BS13" s="39"/>
+      <c r="BT13" s="39"/>
+      <c r="BU13" s="39"/>
+      <c r="BV13" s="39"/>
+      <c r="BW13" s="39"/>
+      <c r="BX13" s="39"/>
+      <c r="BY13" s="39"/>
+      <c r="BZ13" s="39"/>
+      <c r="CA13" s="39"/>
+      <c r="CB13" s="39"/>
+      <c r="CC13" s="39"/>
+      <c r="CD13" s="39"/>
+      <c r="CE13" s="39"/>
+      <c r="CF13" s="39"/>
+      <c r="CG13" s="39"/>
+      <c r="CH13" s="39"/>
+      <c r="CI13" s="39"/>
+      <c r="CJ13" s="39"/>
+      <c r="CK13" s="39"/>
+      <c r="CL13" s="39"/>
+      <c r="CM13" s="39"/>
+      <c r="CN13" s="39"/>
+      <c r="CO13" s="39"/>
+      <c r="CP13" s="39"/>
+      <c r="CQ13" s="39"/>
+      <c r="CR13" s="39"/>
+      <c r="CS13" s="39"/>
+      <c r="CT13" s="39"/>
+      <c r="CU13" s="39"/>
+      <c r="CV13" s="39"/>
+      <c r="CW13" s="39"/>
+      <c r="CX13" s="39"/>
+      <c r="CY13" s="39"/>
+      <c r="CZ13" s="39"/>
+      <c r="DA13" s="39"/>
+      <c r="DB13" s="39"/>
+      <c r="DC13" s="39"/>
+      <c r="DD13" s="39"/>
+      <c r="DE13" s="39"/>
+      <c r="DF13" s="39"/>
+      <c r="DG13" s="39"/>
+      <c r="DH13" s="39"/>
+      <c r="DI13" s="39"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="53"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
+    <row r="14" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="66"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="H14" s="17" t="str">
+        <f t="shared" si="44"/>
+        <v/>
+      </c>
       <c r="I14" s="39"/>
       <c r="J14" s="39"/>
       <c r="K14" s="39"/>
@@ -2642,7 +3611,7 @@
       <c r="V14" s="39"/>
       <c r="W14" s="39"/>
       <c r="X14" s="39"/>
-      <c r="Y14" s="40"/>
+      <c r="Y14" s="39"/>
       <c r="Z14" s="39"/>
       <c r="AA14" s="39"/>
       <c r="AB14" s="39"/>
@@ -2682,16 +3651,78 @@
       <c r="BJ14" s="39"/>
       <c r="BK14" s="39"/>
       <c r="BL14" s="39"/>
+      <c r="BM14" s="39"/>
+      <c r="BN14" s="39"/>
+      <c r="BO14" s="39"/>
+      <c r="BP14" s="39"/>
+      <c r="BQ14" s="39"/>
+      <c r="BR14" s="39"/>
+      <c r="BS14" s="39"/>
+      <c r="BT14" s="39"/>
+      <c r="BU14" s="39"/>
+      <c r="BV14" s="39"/>
+      <c r="BW14" s="39"/>
+      <c r="BX14" s="39"/>
+      <c r="BY14" s="39"/>
+      <c r="BZ14" s="39"/>
+      <c r="CA14" s="39"/>
+      <c r="CB14" s="39"/>
+      <c r="CC14" s="39"/>
+      <c r="CD14" s="39"/>
+      <c r="CE14" s="39"/>
+      <c r="CF14" s="39"/>
+      <c r="CG14" s="39"/>
+      <c r="CH14" s="39"/>
+      <c r="CI14" s="39"/>
+      <c r="CJ14" s="39"/>
+      <c r="CK14" s="39"/>
+      <c r="CL14" s="39"/>
+      <c r="CM14" s="39"/>
+      <c r="CN14" s="39"/>
+      <c r="CO14" s="39"/>
+      <c r="CP14" s="39"/>
+      <c r="CQ14" s="39"/>
+      <c r="CR14" s="39"/>
+      <c r="CS14" s="39"/>
+      <c r="CT14" s="39"/>
+      <c r="CU14" s="39"/>
+      <c r="CV14" s="39"/>
+      <c r="CW14" s="39"/>
+      <c r="CX14" s="39"/>
+      <c r="CY14" s="39"/>
+      <c r="CZ14" s="39"/>
+      <c r="DA14" s="39"/>
+      <c r="DB14" s="39"/>
+      <c r="DC14" s="39"/>
+      <c r="DD14" s="39"/>
+      <c r="DE14" s="39"/>
+      <c r="DF14" s="39"/>
+      <c r="DG14" s="39"/>
+      <c r="DH14" s="39"/>
+      <c r="DI14" s="39"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="53"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
+    <row r="15" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="54"/>
+      <c r="B15" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="67"/>
+      <c r="D15" s="27">
+        <v>0</v>
+      </c>
+      <c r="E15" s="61">
+        <f>F13</f>
+        <v>44913</v>
+      </c>
+      <c r="F15" s="61">
+        <f>E15+15</f>
+        <v>44928</v>
+      </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
+      <c r="H15" s="17">
+        <f t="shared" si="44"/>
+        <v>16</v>
+      </c>
       <c r="I15" s="39"/>
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
@@ -2708,7 +3739,7 @@
       <c r="V15" s="39"/>
       <c r="W15" s="39"/>
       <c r="X15" s="39"/>
-      <c r="Y15" s="40"/>
+      <c r="Y15" s="39"/>
       <c r="Z15" s="39"/>
       <c r="AA15" s="39"/>
       <c r="AB15" s="39"/>
@@ -2748,26 +3779,77 @@
       <c r="BJ15" s="39"/>
       <c r="BK15" s="39"/>
       <c r="BL15" s="39"/>
+      <c r="BM15" s="39"/>
+      <c r="BN15" s="39"/>
+      <c r="BO15" s="39"/>
+      <c r="BP15" s="39"/>
+      <c r="BQ15" s="39"/>
+      <c r="BR15" s="39"/>
+      <c r="BS15" s="39"/>
+      <c r="BT15" s="39"/>
+      <c r="BU15" s="39"/>
+      <c r="BV15" s="39"/>
+      <c r="BW15" s="39"/>
+      <c r="BX15" s="39"/>
+      <c r="BY15" s="39"/>
+      <c r="BZ15" s="39"/>
+      <c r="CA15" s="39"/>
+      <c r="CB15" s="39"/>
+      <c r="CC15" s="39"/>
+      <c r="CD15" s="39"/>
+      <c r="CE15" s="39"/>
+      <c r="CF15" s="39"/>
+      <c r="CG15" s="39"/>
+      <c r="CH15" s="39"/>
+      <c r="CI15" s="39"/>
+      <c r="CJ15" s="39"/>
+      <c r="CK15" s="39"/>
+      <c r="CL15" s="39"/>
+      <c r="CM15" s="39"/>
+      <c r="CN15" s="39"/>
+      <c r="CO15" s="39"/>
+      <c r="CP15" s="39"/>
+      <c r="CQ15" s="39"/>
+      <c r="CR15" s="39"/>
+      <c r="CS15" s="39"/>
+      <c r="CT15" s="39"/>
+      <c r="CU15" s="39"/>
+      <c r="CV15" s="39"/>
+      <c r="CW15" s="39"/>
+      <c r="CX15" s="39"/>
+      <c r="CY15" s="39"/>
+      <c r="CZ15" s="39"/>
+      <c r="DA15" s="39"/>
+      <c r="DB15" s="39"/>
+      <c r="DC15" s="39"/>
+      <c r="DD15" s="39"/>
+      <c r="DE15" s="39"/>
+      <c r="DF15" s="39"/>
+      <c r="DG15" s="39"/>
+      <c r="DH15" s="39"/>
+      <c r="DI15" s="39"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="53"/>
-      <c r="B16" s="71" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="65"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="60">
-        <f>E10+1</f>
-        <v>44869</v>
-      </c>
-      <c r="F16" s="60">
-        <f>E16+2</f>
-        <v>44871</v>
+      <c r="B16" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="67"/>
+      <c r="D16" s="27">
+        <v>0</v>
+      </c>
+      <c r="E16" s="61">
+        <f>F15</f>
+        <v>44928</v>
+      </c>
+      <c r="F16" s="61">
+        <f>E16+10</f>
+        <v>44938</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="44"/>
+        <v>11</v>
       </c>
       <c r="I16" s="39"/>
       <c r="J16" s="39"/>
@@ -2781,8 +3863,8 @@
       <c r="R16" s="39"/>
       <c r="S16" s="39"/>
       <c r="T16" s="39"/>
-      <c r="U16" s="39"/>
-      <c r="V16" s="39"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="40"/>
       <c r="W16" s="39"/>
       <c r="X16" s="39"/>
       <c r="Y16" s="39"/>
@@ -2825,22 +3907,75 @@
       <c r="BJ16" s="39"/>
       <c r="BK16" s="39"/>
       <c r="BL16" s="39"/>
+      <c r="BM16" s="39"/>
+      <c r="BN16" s="39"/>
+      <c r="BO16" s="39"/>
+      <c r="BP16" s="39"/>
+      <c r="BQ16" s="39"/>
+      <c r="BR16" s="39"/>
+      <c r="BS16" s="39"/>
+      <c r="BT16" s="39"/>
+      <c r="BU16" s="39"/>
+      <c r="BV16" s="39"/>
+      <c r="BW16" s="39"/>
+      <c r="BX16" s="39"/>
+      <c r="BY16" s="39"/>
+      <c r="BZ16" s="39"/>
+      <c r="CA16" s="39"/>
+      <c r="CB16" s="39"/>
+      <c r="CC16" s="39"/>
+      <c r="CD16" s="39"/>
+      <c r="CE16" s="39"/>
+      <c r="CF16" s="39"/>
+      <c r="CG16" s="39"/>
+      <c r="CH16" s="39"/>
+      <c r="CI16" s="39"/>
+      <c r="CJ16" s="39"/>
+      <c r="CK16" s="39"/>
+      <c r="CL16" s="39"/>
+      <c r="CM16" s="39"/>
+      <c r="CN16" s="39"/>
+      <c r="CO16" s="39"/>
+      <c r="CP16" s="39"/>
+      <c r="CQ16" s="39"/>
+      <c r="CR16" s="39"/>
+      <c r="CS16" s="39"/>
+      <c r="CT16" s="39"/>
+      <c r="CU16" s="39"/>
+      <c r="CV16" s="39"/>
+      <c r="CW16" s="39"/>
+      <c r="CX16" s="39"/>
+      <c r="CY16" s="39"/>
+      <c r="CZ16" s="39"/>
+      <c r="DA16" s="39"/>
+      <c r="DB16" s="39"/>
+      <c r="DC16" s="39"/>
+      <c r="DD16" s="39"/>
+      <c r="DE16" s="39"/>
+      <c r="DF16" s="39"/>
+      <c r="DG16" s="39"/>
+      <c r="DH16" s="39"/>
+      <c r="DI16" s="39"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
+    <row r="17" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="53"/>
+      <c r="B17" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="67"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="61">
+        <f>F16</f>
+        <v>44938</v>
+      </c>
+      <c r="F17" s="61">
+        <f>E17+3</f>
+        <v>44941</v>
+      </c>
       <c r="G17" s="17"/>
-      <c r="H17" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="H17" s="17">
+        <f t="shared" si="44"/>
+        <v>4</v>
       </c>
       <c r="I17" s="39"/>
       <c r="J17" s="39"/>
@@ -2898,28 +4033,75 @@
       <c r="BJ17" s="39"/>
       <c r="BK17" s="39"/>
       <c r="BL17" s="39"/>
+      <c r="BM17" s="39"/>
+      <c r="BN17" s="39"/>
+      <c r="BO17" s="39"/>
+      <c r="BP17" s="39"/>
+      <c r="BQ17" s="39"/>
+      <c r="BR17" s="39"/>
+      <c r="BS17" s="39"/>
+      <c r="BT17" s="39"/>
+      <c r="BU17" s="39"/>
+      <c r="BV17" s="39"/>
+      <c r="BW17" s="39"/>
+      <c r="BX17" s="39"/>
+      <c r="BY17" s="39"/>
+      <c r="BZ17" s="39"/>
+      <c r="CA17" s="39"/>
+      <c r="CB17" s="39"/>
+      <c r="CC17" s="39"/>
+      <c r="CD17" s="39"/>
+      <c r="CE17" s="39"/>
+      <c r="CF17" s="39"/>
+      <c r="CG17" s="39"/>
+      <c r="CH17" s="39"/>
+      <c r="CI17" s="39"/>
+      <c r="CJ17" s="39"/>
+      <c r="CK17" s="39"/>
+      <c r="CL17" s="39"/>
+      <c r="CM17" s="39"/>
+      <c r="CN17" s="39"/>
+      <c r="CO17" s="39"/>
+      <c r="CP17" s="39"/>
+      <c r="CQ17" s="39"/>
+      <c r="CR17" s="39"/>
+      <c r="CS17" s="39"/>
+      <c r="CT17" s="39"/>
+      <c r="CU17" s="39"/>
+      <c r="CV17" s="39"/>
+      <c r="CW17" s="39"/>
+      <c r="CX17" s="39"/>
+      <c r="CY17" s="39"/>
+      <c r="CZ17" s="39"/>
+      <c r="DA17" s="39"/>
+      <c r="DB17" s="39"/>
+      <c r="DC17" s="39"/>
+      <c r="DD17" s="39"/>
+      <c r="DE17" s="39"/>
+      <c r="DF17" s="39"/>
+      <c r="DG17" s="39"/>
+      <c r="DH17" s="39"/>
+      <c r="DI17" s="39"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
+    <row r="18" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="53"/>
       <c r="B18" s="72" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="67"/>
-      <c r="D18" s="27">
-        <v>0.5</v>
-      </c>
+      <c r="D18" s="27"/>
       <c r="E18" s="61">
-        <f>E16+1</f>
-        <v>44870</v>
+        <f>F16</f>
+        <v>44938</v>
       </c>
       <c r="F18" s="61">
-        <f>E18+4</f>
-        <v>44874</v>
+        <f>E18+10</f>
+        <v>44948</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17">
-        <f t="shared" si="6"/>
-        <v>5</v>
+        <f t="shared" si="44"/>
+        <v>11</v>
       </c>
       <c r="I18" s="39"/>
       <c r="J18" s="39"/>
@@ -2937,7 +4119,7 @@
       <c r="V18" s="39"/>
       <c r="W18" s="39"/>
       <c r="X18" s="39"/>
-      <c r="Y18" s="39"/>
+      <c r="Y18" s="40"/>
       <c r="Z18" s="39"/>
       <c r="AA18" s="39"/>
       <c r="AB18" s="39"/>
@@ -2977,28 +4159,75 @@
       <c r="BJ18" s="39"/>
       <c r="BK18" s="39"/>
       <c r="BL18" s="39"/>
+      <c r="BM18" s="39"/>
+      <c r="BN18" s="39"/>
+      <c r="BO18" s="39"/>
+      <c r="BP18" s="39"/>
+      <c r="BQ18" s="39"/>
+      <c r="BR18" s="39"/>
+      <c r="BS18" s="39"/>
+      <c r="BT18" s="39"/>
+      <c r="BU18" s="39"/>
+      <c r="BV18" s="39"/>
+      <c r="BW18" s="39"/>
+      <c r="BX18" s="39"/>
+      <c r="BY18" s="39"/>
+      <c r="BZ18" s="39"/>
+      <c r="CA18" s="39"/>
+      <c r="CB18" s="39"/>
+      <c r="CC18" s="39"/>
+      <c r="CD18" s="39"/>
+      <c r="CE18" s="39"/>
+      <c r="CF18" s="39"/>
+      <c r="CG18" s="39"/>
+      <c r="CH18" s="39"/>
+      <c r="CI18" s="39"/>
+      <c r="CJ18" s="39"/>
+      <c r="CK18" s="39"/>
+      <c r="CL18" s="39"/>
+      <c r="CM18" s="39"/>
+      <c r="CN18" s="39"/>
+      <c r="CO18" s="39"/>
+      <c r="CP18" s="39"/>
+      <c r="CQ18" s="39"/>
+      <c r="CR18" s="39"/>
+      <c r="CS18" s="39"/>
+      <c r="CT18" s="39"/>
+      <c r="CU18" s="39"/>
+      <c r="CV18" s="39"/>
+      <c r="CW18" s="39"/>
+      <c r="CX18" s="39"/>
+      <c r="CY18" s="39"/>
+      <c r="CZ18" s="39"/>
+      <c r="DA18" s="39"/>
+      <c r="DB18" s="39"/>
+      <c r="DC18" s="39"/>
+      <c r="DD18" s="39"/>
+      <c r="DE18" s="39"/>
+      <c r="DF18" s="39"/>
+      <c r="DG18" s="39"/>
+      <c r="DH18" s="39"/>
+      <c r="DI18" s="39"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="53"/>
       <c r="B19" s="72" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="C19" s="67"/>
-      <c r="D19" s="27">
-        <v>0.5</v>
-      </c>
+      <c r="D19" s="27"/>
       <c r="E19" s="61">
-        <f>E18+2</f>
-        <v>44872</v>
+        <f>E18</f>
+        <v>44938</v>
       </c>
       <c r="F19" s="61">
-        <f>E19+5</f>
-        <v>44877</v>
+        <f>E19+3</f>
+        <v>44941</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17">
-        <f t="shared" si="6"/>
-        <v>6</v>
+        <f t="shared" si="44"/>
+        <v>4</v>
       </c>
       <c r="I19" s="39"/>
       <c r="J19" s="39"/>
@@ -3012,8 +4241,8 @@
       <c r="R19" s="39"/>
       <c r="S19" s="39"/>
       <c r="T19" s="39"/>
-      <c r="U19" s="40"/>
-      <c r="V19" s="40"/>
+      <c r="U19" s="39"/>
+      <c r="V19" s="39"/>
       <c r="W19" s="39"/>
       <c r="X19" s="39"/>
       <c r="Y19" s="39"/>
@@ -3056,26 +4285,71 @@
       <c r="BJ19" s="39"/>
       <c r="BK19" s="39"/>
       <c r="BL19" s="39"/>
+      <c r="BM19" s="39"/>
+      <c r="BN19" s="39"/>
+      <c r="BO19" s="39"/>
+      <c r="BP19" s="39"/>
+      <c r="BQ19" s="39"/>
+      <c r="BR19" s="39"/>
+      <c r="BS19" s="39"/>
+      <c r="BT19" s="39"/>
+      <c r="BU19" s="39"/>
+      <c r="BV19" s="39"/>
+      <c r="BW19" s="39"/>
+      <c r="BX19" s="39"/>
+      <c r="BY19" s="39"/>
+      <c r="BZ19" s="39"/>
+      <c r="CA19" s="39"/>
+      <c r="CB19" s="39"/>
+      <c r="CC19" s="39"/>
+      <c r="CD19" s="39"/>
+      <c r="CE19" s="39"/>
+      <c r="CF19" s="39"/>
+      <c r="CG19" s="39"/>
+      <c r="CH19" s="39"/>
+      <c r="CI19" s="39"/>
+      <c r="CJ19" s="39"/>
+      <c r="CK19" s="39"/>
+      <c r="CL19" s="39"/>
+      <c r="CM19" s="39"/>
+      <c r="CN19" s="39"/>
+      <c r="CO19" s="39"/>
+      <c r="CP19" s="39"/>
+      <c r="CQ19" s="39"/>
+      <c r="CR19" s="39"/>
+      <c r="CS19" s="39"/>
+      <c r="CT19" s="39"/>
+      <c r="CU19" s="39"/>
+      <c r="CV19" s="39"/>
+      <c r="CW19" s="39"/>
+      <c r="CX19" s="39"/>
+      <c r="CY19" s="39"/>
+      <c r="CZ19" s="39"/>
+      <c r="DA19" s="39"/>
+      <c r="DB19" s="39"/>
+      <c r="DC19" s="39"/>
+      <c r="DD19" s="39"/>
+      <c r="DE19" s="39"/>
+      <c r="DF19" s="39"/>
+      <c r="DG19" s="39"/>
+      <c r="DH19" s="39"/>
+      <c r="DI19" s="39"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53"/>
-      <c r="B20" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="61">
-        <f>F19</f>
-        <v>44877</v>
-      </c>
-      <c r="F20" s="61">
-        <f>E20+3</f>
-        <v>44880</v>
-      </c>
+    <row r="20" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="68"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="17"/>
-      <c r="H20" s="17">
-        <f t="shared" si="6"/>
-        <v>4</v>
+      <c r="H20" s="17" t="str">
+        <f t="shared" si="44"/>
+        <v/>
       </c>
       <c r="I20" s="39"/>
       <c r="J20" s="39"/>
@@ -3133,26 +4407,75 @@
       <c r="BJ20" s="39"/>
       <c r="BK20" s="39"/>
       <c r="BL20" s="39"/>
+      <c r="BM20" s="39"/>
+      <c r="BN20" s="39"/>
+      <c r="BO20" s="39"/>
+      <c r="BP20" s="39"/>
+      <c r="BQ20" s="39"/>
+      <c r="BR20" s="39"/>
+      <c r="BS20" s="39"/>
+      <c r="BT20" s="39"/>
+      <c r="BU20" s="39"/>
+      <c r="BV20" s="39"/>
+      <c r="BW20" s="39"/>
+      <c r="BX20" s="39"/>
+      <c r="BY20" s="39"/>
+      <c r="BZ20" s="39"/>
+      <c r="CA20" s="39"/>
+      <c r="CB20" s="39"/>
+      <c r="CC20" s="39"/>
+      <c r="CD20" s="39"/>
+      <c r="CE20" s="39"/>
+      <c r="CF20" s="39"/>
+      <c r="CG20" s="39"/>
+      <c r="CH20" s="39"/>
+      <c r="CI20" s="39"/>
+      <c r="CJ20" s="39"/>
+      <c r="CK20" s="39"/>
+      <c r="CL20" s="39"/>
+      <c r="CM20" s="39"/>
+      <c r="CN20" s="39"/>
+      <c r="CO20" s="39"/>
+      <c r="CP20" s="39"/>
+      <c r="CQ20" s="39"/>
+      <c r="CR20" s="39"/>
+      <c r="CS20" s="39"/>
+      <c r="CT20" s="39"/>
+      <c r="CU20" s="39"/>
+      <c r="CV20" s="39"/>
+      <c r="CW20" s="39"/>
+      <c r="CX20" s="39"/>
+      <c r="CY20" s="39"/>
+      <c r="CZ20" s="39"/>
+      <c r="DA20" s="39"/>
+      <c r="DB20" s="39"/>
+      <c r="DC20" s="39"/>
+      <c r="DD20" s="39"/>
+      <c r="DE20" s="39"/>
+      <c r="DF20" s="39"/>
+      <c r="DG20" s="39"/>
+      <c r="DH20" s="39"/>
+      <c r="DI20" s="39"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="53"/>
-      <c r="B21" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="61">
-        <f>E20</f>
-        <v>44877</v>
-      </c>
-      <c r="F21" s="61">
-        <f>E21+2</f>
-        <v>44879</v>
+      <c r="B21" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="69"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="62">
+        <f>F19</f>
+        <v>44941</v>
+      </c>
+      <c r="F21" s="62">
+        <f>E21+5</f>
+        <v>44946</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17">
-        <f t="shared" si="6"/>
-        <v>3</v>
+        <f t="shared" si="44"/>
+        <v>6</v>
       </c>
       <c r="I21" s="39"/>
       <c r="J21" s="39"/>
@@ -3170,7 +4493,7 @@
       <c r="V21" s="39"/>
       <c r="W21" s="39"/>
       <c r="X21" s="39"/>
-      <c r="Y21" s="40"/>
+      <c r="Y21" s="39"/>
       <c r="Z21" s="39"/>
       <c r="AA21" s="39"/>
       <c r="AB21" s="39"/>
@@ -3210,26 +4533,75 @@
       <c r="BJ21" s="39"/>
       <c r="BK21" s="39"/>
       <c r="BL21" s="39"/>
+      <c r="BM21" s="39"/>
+      <c r="BN21" s="39"/>
+      <c r="BO21" s="39"/>
+      <c r="BP21" s="39"/>
+      <c r="BQ21" s="39"/>
+      <c r="BR21" s="39"/>
+      <c r="BS21" s="39"/>
+      <c r="BT21" s="39"/>
+      <c r="BU21" s="39"/>
+      <c r="BV21" s="39"/>
+      <c r="BW21" s="39"/>
+      <c r="BX21" s="39"/>
+      <c r="BY21" s="39"/>
+      <c r="BZ21" s="39"/>
+      <c r="CA21" s="39"/>
+      <c r="CB21" s="39"/>
+      <c r="CC21" s="39"/>
+      <c r="CD21" s="39"/>
+      <c r="CE21" s="39"/>
+      <c r="CF21" s="39"/>
+      <c r="CG21" s="39"/>
+      <c r="CH21" s="39"/>
+      <c r="CI21" s="39"/>
+      <c r="CJ21" s="39"/>
+      <c r="CK21" s="39"/>
+      <c r="CL21" s="39"/>
+      <c r="CM21" s="39"/>
+      <c r="CN21" s="39"/>
+      <c r="CO21" s="39"/>
+      <c r="CP21" s="39"/>
+      <c r="CQ21" s="39"/>
+      <c r="CR21" s="39"/>
+      <c r="CS21" s="39"/>
+      <c r="CT21" s="39"/>
+      <c r="CU21" s="39"/>
+      <c r="CV21" s="39"/>
+      <c r="CW21" s="39"/>
+      <c r="CX21" s="39"/>
+      <c r="CY21" s="39"/>
+      <c r="CZ21" s="39"/>
+      <c r="DA21" s="39"/>
+      <c r="DB21" s="39"/>
+      <c r="DC21" s="39"/>
+      <c r="DD21" s="39"/>
+      <c r="DE21" s="39"/>
+      <c r="DF21" s="39"/>
+      <c r="DG21" s="39"/>
+      <c r="DH21" s="39"/>
+      <c r="DI21" s="39"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="53"/>
-      <c r="B22" s="72" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="61">
-        <f>E21</f>
-        <v>44877</v>
-      </c>
-      <c r="F22" s="61">
-        <f>E22+3</f>
-        <v>44880</v>
+      <c r="B22" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="69"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="62">
+        <f>F21+1</f>
+        <v>44947</v>
+      </c>
+      <c r="F22" s="62">
+        <f>E22+4</f>
+        <v>44951</v>
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="17">
-        <f t="shared" si="6"/>
-        <v>4</v>
+        <f t="shared" si="44"/>
+        <v>5</v>
       </c>
       <c r="I22" s="39"/>
       <c r="J22" s="39"/>
@@ -3287,22 +4659,73 @@
       <c r="BJ22" s="39"/>
       <c r="BK22" s="39"/>
       <c r="BL22" s="39"/>
+      <c r="BM22" s="39"/>
+      <c r="BN22" s="39"/>
+      <c r="BO22" s="39"/>
+      <c r="BP22" s="39"/>
+      <c r="BQ22" s="39"/>
+      <c r="BR22" s="39"/>
+      <c r="BS22" s="39"/>
+      <c r="BT22" s="39"/>
+      <c r="BU22" s="39"/>
+      <c r="BV22" s="39"/>
+      <c r="BW22" s="39"/>
+      <c r="BX22" s="39"/>
+      <c r="BY22" s="39"/>
+      <c r="BZ22" s="39"/>
+      <c r="CA22" s="39"/>
+      <c r="CB22" s="39"/>
+      <c r="CC22" s="39"/>
+      <c r="CD22" s="39"/>
+      <c r="CE22" s="39"/>
+      <c r="CF22" s="39"/>
+      <c r="CG22" s="39"/>
+      <c r="CH22" s="39"/>
+      <c r="CI22" s="39"/>
+      <c r="CJ22" s="39"/>
+      <c r="CK22" s="39"/>
+      <c r="CL22" s="39"/>
+      <c r="CM22" s="39"/>
+      <c r="CN22" s="39"/>
+      <c r="CO22" s="39"/>
+      <c r="CP22" s="39"/>
+      <c r="CQ22" s="39"/>
+      <c r="CR22" s="39"/>
+      <c r="CS22" s="39"/>
+      <c r="CT22" s="39"/>
+      <c r="CU22" s="39"/>
+      <c r="CV22" s="39"/>
+      <c r="CW22" s="39"/>
+      <c r="CX22" s="39"/>
+      <c r="CY22" s="39"/>
+      <c r="CZ22" s="39"/>
+      <c r="DA22" s="39"/>
+      <c r="DB22" s="39"/>
+      <c r="DC22" s="39"/>
+      <c r="DD22" s="39"/>
+      <c r="DE22" s="39"/>
+      <c r="DF22" s="39"/>
+      <c r="DG22" s="39"/>
+      <c r="DH22" s="39"/>
+      <c r="DI22" s="39"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
+    <row r="23" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="53"/>
+      <c r="B23" s="73"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="62">
+        <f>E22+5</f>
+        <v>44952</v>
+      </c>
+      <c r="F23" s="62">
+        <f>E23+5</f>
+        <v>44957</v>
+      </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
+      <c r="H23" s="17">
+        <f t="shared" si="44"/>
+        <v>6</v>
       </c>
       <c r="I23" s="39"/>
       <c r="J23" s="39"/>
@@ -3360,26 +4783,67 @@
       <c r="BJ23" s="39"/>
       <c r="BK23" s="39"/>
       <c r="BL23" s="39"/>
+      <c r="BM23" s="39"/>
+      <c r="BN23" s="39"/>
+      <c r="BO23" s="39"/>
+      <c r="BP23" s="39"/>
+      <c r="BQ23" s="39"/>
+      <c r="BR23" s="39"/>
+      <c r="BS23" s="39"/>
+      <c r="BT23" s="39"/>
+      <c r="BU23" s="39"/>
+      <c r="BV23" s="39"/>
+      <c r="BW23" s="39"/>
+      <c r="BX23" s="39"/>
+      <c r="BY23" s="39"/>
+      <c r="BZ23" s="39"/>
+      <c r="CA23" s="39"/>
+      <c r="CB23" s="39"/>
+      <c r="CC23" s="39"/>
+      <c r="CD23" s="39"/>
+      <c r="CE23" s="39"/>
+      <c r="CF23" s="39"/>
+      <c r="CG23" s="39"/>
+      <c r="CH23" s="39"/>
+      <c r="CI23" s="39"/>
+      <c r="CJ23" s="39"/>
+      <c r="CK23" s="39"/>
+      <c r="CL23" s="39"/>
+      <c r="CM23" s="39"/>
+      <c r="CN23" s="39"/>
+      <c r="CO23" s="39"/>
+      <c r="CP23" s="39"/>
+      <c r="CQ23" s="39"/>
+      <c r="CR23" s="39"/>
+      <c r="CS23" s="39"/>
+      <c r="CT23" s="39"/>
+      <c r="CU23" s="39"/>
+      <c r="CV23" s="39"/>
+      <c r="CW23" s="39"/>
+      <c r="CX23" s="39"/>
+      <c r="CY23" s="39"/>
+      <c r="CZ23" s="39"/>
+      <c r="DA23" s="39"/>
+      <c r="DB23" s="39"/>
+      <c r="DC23" s="39"/>
+      <c r="DD23" s="39"/>
+      <c r="DE23" s="39"/>
+      <c r="DF23" s="39"/>
+      <c r="DG23" s="39"/>
+      <c r="DH23" s="39"/>
+      <c r="DI23" s="39"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="53"/>
-      <c r="B24" s="73" t="s">
-        <v>3</v>
-      </c>
+      <c r="B24" s="73"/>
       <c r="C24" s="69"/>
       <c r="D24" s="32"/>
-      <c r="E24" s="62">
-        <f>E9+15</f>
-        <v>44880</v>
-      </c>
-      <c r="F24" s="62">
-        <f>E24+5</f>
-        <v>44885</v>
-      </c>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="17"/>
-      <c r="H24" s="17">
-        <f t="shared" si="6"/>
-        <v>6</v>
+      <c r="H24" s="17" t="str">
+        <f t="shared" si="44"/>
+        <v/>
       </c>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
@@ -3437,26 +4901,67 @@
       <c r="BJ24" s="39"/>
       <c r="BK24" s="39"/>
       <c r="BL24" s="39"/>
+      <c r="BM24" s="39"/>
+      <c r="BN24" s="39"/>
+      <c r="BO24" s="39"/>
+      <c r="BP24" s="39"/>
+      <c r="BQ24" s="39"/>
+      <c r="BR24" s="39"/>
+      <c r="BS24" s="39"/>
+      <c r="BT24" s="39"/>
+      <c r="BU24" s="39"/>
+      <c r="BV24" s="39"/>
+      <c r="BW24" s="39"/>
+      <c r="BX24" s="39"/>
+      <c r="BY24" s="39"/>
+      <c r="BZ24" s="39"/>
+      <c r="CA24" s="39"/>
+      <c r="CB24" s="39"/>
+      <c r="CC24" s="39"/>
+      <c r="CD24" s="39"/>
+      <c r="CE24" s="39"/>
+      <c r="CF24" s="39"/>
+      <c r="CG24" s="39"/>
+      <c r="CH24" s="39"/>
+      <c r="CI24" s="39"/>
+      <c r="CJ24" s="39"/>
+      <c r="CK24" s="39"/>
+      <c r="CL24" s="39"/>
+      <c r="CM24" s="39"/>
+      <c r="CN24" s="39"/>
+      <c r="CO24" s="39"/>
+      <c r="CP24" s="39"/>
+      <c r="CQ24" s="39"/>
+      <c r="CR24" s="39"/>
+      <c r="CS24" s="39"/>
+      <c r="CT24" s="39"/>
+      <c r="CU24" s="39"/>
+      <c r="CV24" s="39"/>
+      <c r="CW24" s="39"/>
+      <c r="CX24" s="39"/>
+      <c r="CY24" s="39"/>
+      <c r="CZ24" s="39"/>
+      <c r="DA24" s="39"/>
+      <c r="DB24" s="39"/>
+      <c r="DC24" s="39"/>
+      <c r="DD24" s="39"/>
+      <c r="DE24" s="39"/>
+      <c r="DF24" s="39"/>
+      <c r="DG24" s="39"/>
+      <c r="DH24" s="39"/>
+      <c r="DI24" s="39"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>
-      <c r="B25" s="73" t="s">
-        <v>4</v>
-      </c>
+      <c r="B25" s="73"/>
       <c r="C25" s="69"/>
       <c r="D25" s="32"/>
-      <c r="E25" s="62">
-        <f>F24+1</f>
-        <v>44886</v>
-      </c>
-      <c r="F25" s="62">
-        <f>E25+4</f>
-        <v>44890</v>
-      </c>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="17"/>
-      <c r="H25" s="17">
-        <f t="shared" si="6"/>
-        <v>5</v>
+      <c r="H25" s="17" t="str">
+        <f t="shared" si="44"/>
+        <v/>
       </c>
       <c r="I25" s="39"/>
       <c r="J25" s="39"/>
@@ -3514,26 +5019,69 @@
       <c r="BJ25" s="39"/>
       <c r="BK25" s="39"/>
       <c r="BL25" s="39"/>
+      <c r="BM25" s="39"/>
+      <c r="BN25" s="39"/>
+      <c r="BO25" s="39"/>
+      <c r="BP25" s="39"/>
+      <c r="BQ25" s="39"/>
+      <c r="BR25" s="39"/>
+      <c r="BS25" s="39"/>
+      <c r="BT25" s="39"/>
+      <c r="BU25" s="39"/>
+      <c r="BV25" s="39"/>
+      <c r="BW25" s="39"/>
+      <c r="BX25" s="39"/>
+      <c r="BY25" s="39"/>
+      <c r="BZ25" s="39"/>
+      <c r="CA25" s="39"/>
+      <c r="CB25" s="39"/>
+      <c r="CC25" s="39"/>
+      <c r="CD25" s="39"/>
+      <c r="CE25" s="39"/>
+      <c r="CF25" s="39"/>
+      <c r="CG25" s="39"/>
+      <c r="CH25" s="39"/>
+      <c r="CI25" s="39"/>
+      <c r="CJ25" s="39"/>
+      <c r="CK25" s="39"/>
+      <c r="CL25" s="39"/>
+      <c r="CM25" s="39"/>
+      <c r="CN25" s="39"/>
+      <c r="CO25" s="39"/>
+      <c r="CP25" s="39"/>
+      <c r="CQ25" s="39"/>
+      <c r="CR25" s="39"/>
+      <c r="CS25" s="39"/>
+      <c r="CT25" s="39"/>
+      <c r="CU25" s="39"/>
+      <c r="CV25" s="39"/>
+      <c r="CW25" s="39"/>
+      <c r="CX25" s="39"/>
+      <c r="CY25" s="39"/>
+      <c r="CZ25" s="39"/>
+      <c r="DA25" s="39"/>
+      <c r="DB25" s="39"/>
+      <c r="DC25" s="39"/>
+      <c r="DD25" s="39"/>
+      <c r="DE25" s="39"/>
+      <c r="DF25" s="39"/>
+      <c r="DG25" s="39"/>
+      <c r="DH25" s="39"/>
+      <c r="DI25" s="39"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="53"/>
-      <c r="B26" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="69"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="62">
-        <f>E25+5</f>
-        <v>44891</v>
-      </c>
-      <c r="F26" s="62">
-        <f>E26+5</f>
-        <v>44896</v>
-      </c>
+    <row r="26" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
       <c r="G26" s="17"/>
-      <c r="H26" s="17">
-        <f t="shared" si="6"/>
-        <v>6</v>
+      <c r="H26" s="17" t="str">
+        <f t="shared" si="44"/>
+        <v/>
       </c>
       <c r="I26" s="39"/>
       <c r="J26" s="39"/>
@@ -3591,26 +5139,67 @@
       <c r="BJ26" s="39"/>
       <c r="BK26" s="39"/>
       <c r="BL26" s="39"/>
+      <c r="BM26" s="39"/>
+      <c r="BN26" s="39"/>
+      <c r="BO26" s="39"/>
+      <c r="BP26" s="39"/>
+      <c r="BQ26" s="39"/>
+      <c r="BR26" s="39"/>
+      <c r="BS26" s="39"/>
+      <c r="BT26" s="39"/>
+      <c r="BU26" s="39"/>
+      <c r="BV26" s="39"/>
+      <c r="BW26" s="39"/>
+      <c r="BX26" s="39"/>
+      <c r="BY26" s="39"/>
+      <c r="BZ26" s="39"/>
+      <c r="CA26" s="39"/>
+      <c r="CB26" s="39"/>
+      <c r="CC26" s="39"/>
+      <c r="CD26" s="39"/>
+      <c r="CE26" s="39"/>
+      <c r="CF26" s="39"/>
+      <c r="CG26" s="39"/>
+      <c r="CH26" s="39"/>
+      <c r="CI26" s="39"/>
+      <c r="CJ26" s="39"/>
+      <c r="CK26" s="39"/>
+      <c r="CL26" s="39"/>
+      <c r="CM26" s="39"/>
+      <c r="CN26" s="39"/>
+      <c r="CO26" s="39"/>
+      <c r="CP26" s="39"/>
+      <c r="CQ26" s="39"/>
+      <c r="CR26" s="39"/>
+      <c r="CS26" s="39"/>
+      <c r="CT26" s="39"/>
+      <c r="CU26" s="39"/>
+      <c r="CV26" s="39"/>
+      <c r="CW26" s="39"/>
+      <c r="CX26" s="39"/>
+      <c r="CY26" s="39"/>
+      <c r="CZ26" s="39"/>
+      <c r="DA26" s="39"/>
+      <c r="DB26" s="39"/>
+      <c r="DC26" s="39"/>
+      <c r="DD26" s="39"/>
+      <c r="DE26" s="39"/>
+      <c r="DF26" s="39"/>
+      <c r="DG26" s="39"/>
+      <c r="DH26" s="39"/>
+      <c r="DI26" s="39"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="53"/>
-      <c r="B27" s="73" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="69"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="62">
-        <f>F26+1</f>
-        <v>44897</v>
-      </c>
-      <c r="F27" s="62">
-        <f>E27+4</f>
-        <v>44901</v>
-      </c>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
       <c r="G27" s="17"/>
-      <c r="H27" s="17">
-        <f t="shared" si="6"/>
-        <v>5</v>
+      <c r="H27" s="17" t="str">
+        <f t="shared" si="44"/>
+        <v/>
       </c>
       <c r="I27" s="39"/>
       <c r="J27" s="39"/>
@@ -3668,26 +5257,67 @@
       <c r="BJ27" s="39"/>
       <c r="BK27" s="39"/>
       <c r="BL27" s="39"/>
+      <c r="BM27" s="39"/>
+      <c r="BN27" s="39"/>
+      <c r="BO27" s="39"/>
+      <c r="BP27" s="39"/>
+      <c r="BQ27" s="39"/>
+      <c r="BR27" s="39"/>
+      <c r="BS27" s="39"/>
+      <c r="BT27" s="39"/>
+      <c r="BU27" s="39"/>
+      <c r="BV27" s="39"/>
+      <c r="BW27" s="39"/>
+      <c r="BX27" s="39"/>
+      <c r="BY27" s="39"/>
+      <c r="BZ27" s="39"/>
+      <c r="CA27" s="39"/>
+      <c r="CB27" s="39"/>
+      <c r="CC27" s="39"/>
+      <c r="CD27" s="39"/>
+      <c r="CE27" s="39"/>
+      <c r="CF27" s="39"/>
+      <c r="CG27" s="39"/>
+      <c r="CH27" s="39"/>
+      <c r="CI27" s="39"/>
+      <c r="CJ27" s="39"/>
+      <c r="CK27" s="39"/>
+      <c r="CL27" s="39"/>
+      <c r="CM27" s="39"/>
+      <c r="CN27" s="39"/>
+      <c r="CO27" s="39"/>
+      <c r="CP27" s="39"/>
+      <c r="CQ27" s="39"/>
+      <c r="CR27" s="39"/>
+      <c r="CS27" s="39"/>
+      <c r="CT27" s="39"/>
+      <c r="CU27" s="39"/>
+      <c r="CV27" s="39"/>
+      <c r="CW27" s="39"/>
+      <c r="CX27" s="39"/>
+      <c r="CY27" s="39"/>
+      <c r="CZ27" s="39"/>
+      <c r="DA27" s="39"/>
+      <c r="DB27" s="39"/>
+      <c r="DC27" s="39"/>
+      <c r="DD27" s="39"/>
+      <c r="DE27" s="39"/>
+      <c r="DF27" s="39"/>
+      <c r="DG27" s="39"/>
+      <c r="DH27" s="39"/>
+      <c r="DI27" s="39"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="53"/>
-      <c r="B28" s="73" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28" s="69"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="62">
-        <f>E26</f>
-        <v>44891</v>
-      </c>
-      <c r="F28" s="62">
-        <f>E28+4</f>
-        <v>44895</v>
-      </c>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="17">
-        <f t="shared" si="6"/>
-        <v>5</v>
+      <c r="H28" s="17" t="str">
+        <f t="shared" si="44"/>
+        <v/>
       </c>
       <c r="I28" s="39"/>
       <c r="J28" s="39"/>
@@ -3745,11 +5375,58 @@
       <c r="BJ28" s="39"/>
       <c r="BK28" s="39"/>
       <c r="BL28" s="39"/>
+      <c r="BM28" s="39"/>
+      <c r="BN28" s="39"/>
+      <c r="BO28" s="39"/>
+      <c r="BP28" s="39"/>
+      <c r="BQ28" s="39"/>
+      <c r="BR28" s="39"/>
+      <c r="BS28" s="39"/>
+      <c r="BT28" s="39"/>
+      <c r="BU28" s="39"/>
+      <c r="BV28" s="39"/>
+      <c r="BW28" s="39"/>
+      <c r="BX28" s="39"/>
+      <c r="BY28" s="39"/>
+      <c r="BZ28" s="39"/>
+      <c r="CA28" s="39"/>
+      <c r="CB28" s="39"/>
+      <c r="CC28" s="39"/>
+      <c r="CD28" s="39"/>
+      <c r="CE28" s="39"/>
+      <c r="CF28" s="39"/>
+      <c r="CG28" s="39"/>
+      <c r="CH28" s="39"/>
+      <c r="CI28" s="39"/>
+      <c r="CJ28" s="39"/>
+      <c r="CK28" s="39"/>
+      <c r="CL28" s="39"/>
+      <c r="CM28" s="39"/>
+      <c r="CN28" s="39"/>
+      <c r="CO28" s="39"/>
+      <c r="CP28" s="39"/>
+      <c r="CQ28" s="39"/>
+      <c r="CR28" s="39"/>
+      <c r="CS28" s="39"/>
+      <c r="CT28" s="39"/>
+      <c r="CU28" s="39"/>
+      <c r="CV28" s="39"/>
+      <c r="CW28" s="39"/>
+      <c r="CX28" s="39"/>
+      <c r="CY28" s="39"/>
+      <c r="CZ28" s="39"/>
+      <c r="DA28" s="39"/>
+      <c r="DB28" s="39"/>
+      <c r="DC28" s="39"/>
+      <c r="DD28" s="39"/>
+      <c r="DE28" s="39"/>
+      <c r="DF28" s="39"/>
+      <c r="DG28" s="39"/>
+      <c r="DH28" s="39"/>
+      <c r="DI28" s="39"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="53" t="s">
-        <v>31</v>
-      </c>
+    <row r="29" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="53"/>
       <c r="B29" s="70"/>
       <c r="C29" s="70"/>
       <c r="D29" s="70"/>
@@ -3757,7 +5434,7 @@
       <c r="F29" s="70"/>
       <c r="G29" s="17"/>
       <c r="H29" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="I29" s="39"/>
@@ -3816,8 +5493,57 @@
       <c r="BJ29" s="39"/>
       <c r="BK29" s="39"/>
       <c r="BL29" s="39"/>
+      <c r="BM29" s="39"/>
+      <c r="BN29" s="39"/>
+      <c r="BO29" s="39"/>
+      <c r="BP29" s="39"/>
+      <c r="BQ29" s="39"/>
+      <c r="BR29" s="39"/>
+      <c r="BS29" s="39"/>
+      <c r="BT29" s="39"/>
+      <c r="BU29" s="39"/>
+      <c r="BV29" s="39"/>
+      <c r="BW29" s="39"/>
+      <c r="BX29" s="39"/>
+      <c r="BY29" s="39"/>
+      <c r="BZ29" s="39"/>
+      <c r="CA29" s="39"/>
+      <c r="CB29" s="39"/>
+      <c r="CC29" s="39"/>
+      <c r="CD29" s="39"/>
+      <c r="CE29" s="39"/>
+      <c r="CF29" s="39"/>
+      <c r="CG29" s="39"/>
+      <c r="CH29" s="39"/>
+      <c r="CI29" s="39"/>
+      <c r="CJ29" s="39"/>
+      <c r="CK29" s="39"/>
+      <c r="CL29" s="39"/>
+      <c r="CM29" s="39"/>
+      <c r="CN29" s="39"/>
+      <c r="CO29" s="39"/>
+      <c r="CP29" s="39"/>
+      <c r="CQ29" s="39"/>
+      <c r="CR29" s="39"/>
+      <c r="CS29" s="39"/>
+      <c r="CT29" s="39"/>
+      <c r="CU29" s="39"/>
+      <c r="CV29" s="39"/>
+      <c r="CW29" s="39"/>
+      <c r="CX29" s="39"/>
+      <c r="CY29" s="39"/>
+      <c r="CZ29" s="39"/>
+      <c r="DA29" s="39"/>
+      <c r="DB29" s="39"/>
+      <c r="DC29" s="39"/>
+      <c r="DD29" s="39"/>
+      <c r="DE29" s="39"/>
+      <c r="DF29" s="39"/>
+      <c r="DG29" s="39"/>
+      <c r="DH29" s="39"/>
+      <c r="DI29" s="39"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="53"/>
       <c r="B30" s="70"/>
       <c r="C30" s="70"/>
@@ -3826,7 +5552,7 @@
       <c r="F30" s="70"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="I30" s="39"/>
@@ -3885,8 +5611,57 @@
       <c r="BJ30" s="39"/>
       <c r="BK30" s="39"/>
       <c r="BL30" s="39"/>
+      <c r="BM30" s="39"/>
+      <c r="BN30" s="39"/>
+      <c r="BO30" s="39"/>
+      <c r="BP30" s="39"/>
+      <c r="BQ30" s="39"/>
+      <c r="BR30" s="39"/>
+      <c r="BS30" s="39"/>
+      <c r="BT30" s="39"/>
+      <c r="BU30" s="39"/>
+      <c r="BV30" s="39"/>
+      <c r="BW30" s="39"/>
+      <c r="BX30" s="39"/>
+      <c r="BY30" s="39"/>
+      <c r="BZ30" s="39"/>
+      <c r="CA30" s="39"/>
+      <c r="CB30" s="39"/>
+      <c r="CC30" s="39"/>
+      <c r="CD30" s="39"/>
+      <c r="CE30" s="39"/>
+      <c r="CF30" s="39"/>
+      <c r="CG30" s="39"/>
+      <c r="CH30" s="39"/>
+      <c r="CI30" s="39"/>
+      <c r="CJ30" s="39"/>
+      <c r="CK30" s="39"/>
+      <c r="CL30" s="39"/>
+      <c r="CM30" s="39"/>
+      <c r="CN30" s="39"/>
+      <c r="CO30" s="39"/>
+      <c r="CP30" s="39"/>
+      <c r="CQ30" s="39"/>
+      <c r="CR30" s="39"/>
+      <c r="CS30" s="39"/>
+      <c r="CT30" s="39"/>
+      <c r="CU30" s="39"/>
+      <c r="CV30" s="39"/>
+      <c r="CW30" s="39"/>
+      <c r="CX30" s="39"/>
+      <c r="CY30" s="39"/>
+      <c r="CZ30" s="39"/>
+      <c r="DA30" s="39"/>
+      <c r="DB30" s="39"/>
+      <c r="DC30" s="39"/>
+      <c r="DD30" s="39"/>
+      <c r="DE30" s="39"/>
+      <c r="DF30" s="39"/>
+      <c r="DG30" s="39"/>
+      <c r="DH30" s="39"/>
+      <c r="DI30" s="39"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="53"/>
       <c r="B31" s="70"/>
       <c r="C31" s="70"/>
@@ -3895,7 +5670,7 @@
       <c r="F31" s="70"/>
       <c r="G31" s="17"/>
       <c r="H31" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="I31" s="39"/>
@@ -3954,17 +5729,68 @@
       <c r="BJ31" s="39"/>
       <c r="BK31" s="39"/>
       <c r="BL31" s="39"/>
+      <c r="BM31" s="39"/>
+      <c r="BN31" s="39"/>
+      <c r="BO31" s="39"/>
+      <c r="BP31" s="39"/>
+      <c r="BQ31" s="39"/>
+      <c r="BR31" s="39"/>
+      <c r="BS31" s="39"/>
+      <c r="BT31" s="39"/>
+      <c r="BU31" s="39"/>
+      <c r="BV31" s="39"/>
+      <c r="BW31" s="39"/>
+      <c r="BX31" s="39"/>
+      <c r="BY31" s="39"/>
+      <c r="BZ31" s="39"/>
+      <c r="CA31" s="39"/>
+      <c r="CB31" s="39"/>
+      <c r="CC31" s="39"/>
+      <c r="CD31" s="39"/>
+      <c r="CE31" s="39"/>
+      <c r="CF31" s="39"/>
+      <c r="CG31" s="39"/>
+      <c r="CH31" s="39"/>
+      <c r="CI31" s="39"/>
+      <c r="CJ31" s="39"/>
+      <c r="CK31" s="39"/>
+      <c r="CL31" s="39"/>
+      <c r="CM31" s="39"/>
+      <c r="CN31" s="39"/>
+      <c r="CO31" s="39"/>
+      <c r="CP31" s="39"/>
+      <c r="CQ31" s="39"/>
+      <c r="CR31" s="39"/>
+      <c r="CS31" s="39"/>
+      <c r="CT31" s="39"/>
+      <c r="CU31" s="39"/>
+      <c r="CV31" s="39"/>
+      <c r="CW31" s="39"/>
+      <c r="CX31" s="39"/>
+      <c r="CY31" s="39"/>
+      <c r="CZ31" s="39"/>
+      <c r="DA31" s="39"/>
+      <c r="DB31" s="39"/>
+      <c r="DC31" s="39"/>
+      <c r="DD31" s="39"/>
+      <c r="DE31" s="39"/>
+      <c r="DF31" s="39"/>
+      <c r="DG31" s="39"/>
+      <c r="DH31" s="39"/>
+      <c r="DI31" s="39"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="53"/>
-      <c r="B32" s="70"/>
+    <row r="32" spans="1:113" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="74"/>
       <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
       <c r="G32" s="17"/>
       <c r="H32" s="17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="I32" s="39"/>
@@ -4023,301 +5849,148 @@
       <c r="BJ32" s="39"/>
       <c r="BK32" s="39"/>
       <c r="BL32" s="39"/>
+      <c r="BM32" s="39"/>
+      <c r="BN32" s="39"/>
+      <c r="BO32" s="39"/>
+      <c r="BP32" s="39"/>
+      <c r="BQ32" s="39"/>
+      <c r="BR32" s="39"/>
+      <c r="BS32" s="39"/>
+      <c r="BT32" s="39"/>
+      <c r="BU32" s="39"/>
+      <c r="BV32" s="39"/>
+      <c r="BW32" s="39"/>
+      <c r="BX32" s="39"/>
+      <c r="BY32" s="39"/>
+      <c r="BZ32" s="39"/>
+      <c r="CA32" s="39"/>
+      <c r="CB32" s="39"/>
+      <c r="CC32" s="39"/>
+      <c r="CD32" s="39"/>
+      <c r="CE32" s="39"/>
+      <c r="CF32" s="39"/>
+      <c r="CG32" s="39"/>
+      <c r="CH32" s="39"/>
+      <c r="CI32" s="39"/>
+      <c r="CJ32" s="39"/>
+      <c r="CK32" s="39"/>
+      <c r="CL32" s="39"/>
+      <c r="CM32" s="39"/>
+      <c r="CN32" s="39"/>
+      <c r="CO32" s="39"/>
+      <c r="CP32" s="39"/>
+      <c r="CQ32" s="39"/>
+      <c r="CR32" s="39"/>
+      <c r="CS32" s="39"/>
+      <c r="CT32" s="39"/>
+      <c r="CU32" s="39"/>
+      <c r="CV32" s="39"/>
+      <c r="CW32" s="39"/>
+      <c r="CX32" s="39"/>
+      <c r="CY32" s="39"/>
+      <c r="CZ32" s="39"/>
+      <c r="DA32" s="39"/>
+      <c r="DB32" s="39"/>
+      <c r="DC32" s="39"/>
+      <c r="DD32" s="39"/>
+      <c r="DE32" s="39"/>
+      <c r="DF32" s="39"/>
+      <c r="DG32" s="39"/>
+      <c r="DH32" s="39"/>
+      <c r="DI32" s="39"/>
     </row>
     <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="53"/>
-      <c r="B33" s="70"/>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17" t="str">
-        <f t="shared" si="6"/>
+      <c r="A33" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38" t="str">
+        <f t="shared" si="44"/>
         <v/>
       </c>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="39"/>
-      <c r="R33" s="39"/>
-      <c r="S33" s="39"/>
-      <c r="T33" s="39"/>
-      <c r="U33" s="39"/>
-      <c r="V33" s="39"/>
-      <c r="W33" s="39"/>
-      <c r="X33" s="39"/>
-      <c r="Y33" s="39"/>
-      <c r="Z33" s="39"/>
-      <c r="AA33" s="39"/>
-      <c r="AB33" s="39"/>
-      <c r="AC33" s="39"/>
-      <c r="AD33" s="39"/>
-      <c r="AE33" s="39"/>
-      <c r="AF33" s="39"/>
-      <c r="AG33" s="39"/>
-      <c r="AH33" s="39"/>
-      <c r="AI33" s="39"/>
-      <c r="AJ33" s="39"/>
-      <c r="AK33" s="39"/>
-      <c r="AL33" s="39"/>
-      <c r="AM33" s="39"/>
-      <c r="AN33" s="39"/>
-      <c r="AO33" s="39"/>
-      <c r="AP33" s="39"/>
-      <c r="AQ33" s="39"/>
-      <c r="AR33" s="39"/>
-      <c r="AS33" s="39"/>
-      <c r="AT33" s="39"/>
-      <c r="AU33" s="39"/>
-      <c r="AV33" s="39"/>
-      <c r="AW33" s="39"/>
-      <c r="AX33" s="39"/>
-      <c r="AY33" s="39"/>
-      <c r="AZ33" s="39"/>
-      <c r="BA33" s="39"/>
-      <c r="BB33" s="39"/>
-      <c r="BC33" s="39"/>
-      <c r="BD33" s="39"/>
-      <c r="BE33" s="39"/>
-      <c r="BF33" s="39"/>
-      <c r="BG33" s="39"/>
-      <c r="BH33" s="39"/>
-      <c r="BI33" s="39"/>
-      <c r="BJ33" s="39"/>
-      <c r="BK33" s="39"/>
-      <c r="BL33" s="39"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="41"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="41"/>
+      <c r="M33" s="41"/>
+      <c r="N33" s="41"/>
+      <c r="O33" s="41"/>
+      <c r="P33" s="41"/>
+      <c r="Q33" s="41"/>
+      <c r="R33" s="41"/>
+      <c r="S33" s="41"/>
+      <c r="T33" s="41"/>
+      <c r="U33" s="41"/>
+      <c r="V33" s="41"/>
+      <c r="W33" s="41"/>
+      <c r="X33" s="41"/>
+      <c r="Y33" s="41"/>
+      <c r="Z33" s="41"/>
+      <c r="AA33" s="41"/>
+      <c r="AB33" s="41"/>
+      <c r="AC33" s="41"/>
+      <c r="AD33" s="41"/>
+      <c r="AE33" s="41"/>
+      <c r="AF33" s="41"/>
+      <c r="AG33" s="41"/>
+      <c r="AH33" s="41"/>
+      <c r="AI33" s="41"/>
+      <c r="AJ33" s="41"/>
+      <c r="AK33" s="41"/>
+      <c r="AL33" s="41"/>
+      <c r="AM33" s="41"/>
+      <c r="AN33" s="41"/>
+      <c r="AO33" s="41"/>
+      <c r="AP33" s="41"/>
+      <c r="AQ33" s="41"/>
+      <c r="AR33" s="41"/>
+      <c r="AS33" s="41"/>
+      <c r="AT33" s="41"/>
+      <c r="AU33" s="41"/>
+      <c r="AV33" s="41"/>
+      <c r="AW33" s="41"/>
+      <c r="AX33" s="41"/>
+      <c r="AY33" s="41"/>
+      <c r="AZ33" s="41"/>
+      <c r="BA33" s="41"/>
+      <c r="BB33" s="41"/>
+      <c r="BC33" s="41"/>
+      <c r="BD33" s="41"/>
+      <c r="BE33" s="41"/>
+      <c r="BF33" s="41"/>
+      <c r="BG33" s="41"/>
+      <c r="BH33" s="41"/>
+      <c r="BI33" s="41"/>
+      <c r="BJ33" s="41"/>
+      <c r="BK33" s="41"/>
+      <c r="BL33" s="41"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="53"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="39"/>
-      <c r="S34" s="39"/>
-      <c r="T34" s="39"/>
-      <c r="U34" s="39"/>
-      <c r="V34" s="39"/>
-      <c r="W34" s="39"/>
-      <c r="X34" s="39"/>
-      <c r="Y34" s="39"/>
-      <c r="Z34" s="39"/>
-      <c r="AA34" s="39"/>
-      <c r="AB34" s="39"/>
-      <c r="AC34" s="39"/>
-      <c r="AD34" s="39"/>
-      <c r="AE34" s="39"/>
-      <c r="AF34" s="39"/>
-      <c r="AG34" s="39"/>
-      <c r="AH34" s="39"/>
-      <c r="AI34" s="39"/>
-      <c r="AJ34" s="39"/>
-      <c r="AK34" s="39"/>
-      <c r="AL34" s="39"/>
-      <c r="AM34" s="39"/>
-      <c r="AN34" s="39"/>
-      <c r="AO34" s="39"/>
-      <c r="AP34" s="39"/>
-      <c r="AQ34" s="39"/>
-      <c r="AR34" s="39"/>
-      <c r="AS34" s="39"/>
-      <c r="AT34" s="39"/>
-      <c r="AU34" s="39"/>
-      <c r="AV34" s="39"/>
-      <c r="AW34" s="39"/>
-      <c r="AX34" s="39"/>
-      <c r="AY34" s="39"/>
-      <c r="AZ34" s="39"/>
-      <c r="BA34" s="39"/>
-      <c r="BB34" s="39"/>
-      <c r="BC34" s="39"/>
-      <c r="BD34" s="39"/>
-      <c r="BE34" s="39"/>
-      <c r="BF34" s="39"/>
-      <c r="BG34" s="39"/>
-      <c r="BH34" s="39"/>
-      <c r="BI34" s="39"/>
-      <c r="BJ34" s="39"/>
-      <c r="BK34" s="39"/>
-      <c r="BL34" s="39"/>
+    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="74"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="39"/>
-      <c r="R35" s="39"/>
-      <c r="S35" s="39"/>
-      <c r="T35" s="39"/>
-      <c r="U35" s="39"/>
-      <c r="V35" s="39"/>
-      <c r="W35" s="39"/>
-      <c r="X35" s="39"/>
-      <c r="Y35" s="39"/>
-      <c r="Z35" s="39"/>
-      <c r="AA35" s="39"/>
-      <c r="AB35" s="39"/>
-      <c r="AC35" s="39"/>
-      <c r="AD35" s="39"/>
-      <c r="AE35" s="39"/>
-      <c r="AF35" s="39"/>
-      <c r="AG35" s="39"/>
-      <c r="AH35" s="39"/>
-      <c r="AI35" s="39"/>
-      <c r="AJ35" s="39"/>
-      <c r="AK35" s="39"/>
-      <c r="AL35" s="39"/>
-      <c r="AM35" s="39"/>
-      <c r="AN35" s="39"/>
-      <c r="AO35" s="39"/>
-      <c r="AP35" s="39"/>
-      <c r="AQ35" s="39"/>
-      <c r="AR35" s="39"/>
-      <c r="AS35" s="39"/>
-      <c r="AT35" s="39"/>
-      <c r="AU35" s="39"/>
-      <c r="AV35" s="39"/>
-      <c r="AW35" s="39"/>
-      <c r="AX35" s="39"/>
-      <c r="AY35" s="39"/>
-      <c r="AZ35" s="39"/>
-      <c r="BA35" s="39"/>
-      <c r="BB35" s="39"/>
-      <c r="BC35" s="39"/>
-      <c r="BD35" s="39"/>
-      <c r="BE35" s="39"/>
-      <c r="BF35" s="39"/>
-      <c r="BG35" s="39"/>
-      <c r="BH35" s="39"/>
-      <c r="BI35" s="39"/>
-      <c r="BJ35" s="39"/>
-      <c r="BK35" s="39"/>
-      <c r="BL35" s="39"/>
+    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="14"/>
+      <c r="F35" s="55"/>
     </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="41"/>
-      <c r="P36" s="41"/>
-      <c r="Q36" s="41"/>
-      <c r="R36" s="41"/>
-      <c r="S36" s="41"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="41"/>
-      <c r="V36" s="41"/>
-      <c r="W36" s="41"/>
-      <c r="X36" s="41"/>
-      <c r="Y36" s="41"/>
-      <c r="Z36" s="41"/>
-      <c r="AA36" s="41"/>
-      <c r="AB36" s="41"/>
-      <c r="AC36" s="41"/>
-      <c r="AD36" s="41"/>
-      <c r="AE36" s="41"/>
-      <c r="AF36" s="41"/>
-      <c r="AG36" s="41"/>
-      <c r="AH36" s="41"/>
-      <c r="AI36" s="41"/>
-      <c r="AJ36" s="41"/>
-      <c r="AK36" s="41"/>
-      <c r="AL36" s="41"/>
-      <c r="AM36" s="41"/>
-      <c r="AN36" s="41"/>
-      <c r="AO36" s="41"/>
-      <c r="AP36" s="41"/>
-      <c r="AQ36" s="41"/>
-      <c r="AR36" s="41"/>
-      <c r="AS36" s="41"/>
-      <c r="AT36" s="41"/>
-      <c r="AU36" s="41"/>
-      <c r="AV36" s="41"/>
-      <c r="AW36" s="41"/>
-      <c r="AX36" s="41"/>
-      <c r="AY36" s="41"/>
-      <c r="AZ36" s="41"/>
-      <c r="BA36" s="41"/>
-      <c r="BB36" s="41"/>
-      <c r="BC36" s="41"/>
-      <c r="BD36" s="41"/>
-      <c r="BE36" s="41"/>
-      <c r="BF36" s="41"/>
-      <c r="BG36" s="41"/>
-      <c r="BH36" s="41"/>
-      <c r="BI36" s="41"/>
-      <c r="BJ36" s="41"/>
-      <c r="BK36" s="41"/>
-      <c r="BL36" s="41"/>
-    </row>
-    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" s="14"/>
-      <c r="F38" s="55"/>
-    </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="15"/>
+    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="18">
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
@@ -4330,8 +6003,8 @@
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D36">
-    <cfRule type="dataBar" priority="14">
+  <conditionalFormatting sqref="D7:D33">
+    <cfRule type="dataBar" priority="27">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4344,17 +6017,76 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL36">
-    <cfRule type="expression" dxfId="2" priority="33">
+  <conditionalFormatting sqref="I5:BL33 BM8:BZ13 BM14:DI32">
+    <cfRule type="expression" dxfId="15" priority="46">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL36">
-    <cfRule type="expression" dxfId="1" priority="27">
+  <conditionalFormatting sqref="I7:BL33 BM8:BZ13 BM14:DI32">
+    <cfRule type="expression" dxfId="14" priority="40">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="41" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM5:BZ6">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CA8:CN13">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CA8:CN13">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>AND(task_start&lt;=CA$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CA$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+      <formula>AND(task_end&gt;=CA$5,task_start&lt;CB$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CA5:CN6">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>AND(TODAY()&gt;=CA$5,TODAY()&lt;CB$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CO8:DB13">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CO8:DB13">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>AND(task_start&lt;=CO$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=CO$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+      <formula>AND(task_end&gt;=CO$5,task_start&lt;CP$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CO5:DB6">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>AND(TODAY()&gt;=CO$5,TODAY()&lt;CP$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DC8:DI13">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>AND(TODAY()&gt;=DC$5,TODAY()&lt;DD$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DC8:DI13">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>AND(task_start&lt;=DC$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=DC$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+      <formula>AND(task_end&gt;=DC$5,task_start&lt;DD$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="DC5:DI6">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(TODAY()&gt;=DC$5,TODAY()&lt;DD$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4369,7 +6101,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F21 F25:F26 E26" formula="1"/>
+    <ignoredError sqref="F22:F23 E23" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4387,7 +6119,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D36</xm:sqref>
+          <xm:sqref>D7:D33</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4410,79 +6142,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="45" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="44"/>
     </row>
     <row r="3" spans="1:2" s="49" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="78" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" s="50"/>
     </row>
     <row r="4" spans="1:2" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="47" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="48" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="47" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="43" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="47" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="48" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="43" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="47" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="48" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="43" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="51" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="46" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="47" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="48" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>